<commit_message>
Implement edit selection features, update readme, and fix total income/expense bu
</commit_message>
<xml_diff>
--- a/budget_data.xlsx
+++ b/budget_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,26 +446,13 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
           <t>asd</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>1</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix formatting bugs and updated readme
</commit_message>
<xml_diff>
--- a/budget_data.xlsx
+++ b/budget_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,12 +446,29 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>asfd</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>$12.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>efa</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$1.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update methods to work in memory instead of excel
</commit_message>
<xml_diff>
--- a/budget_data.xlsx
+++ b/budget_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,40 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Income</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>asfd</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>$12.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Income</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>efa</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>$1.00</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update to use context manager, file ready for merge
</commit_message>
<xml_diff>
--- a/budget_data.xlsx
+++ b/budget_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,108 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>$123.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2we2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$2.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>$222.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$22.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$22.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$100.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>